<commit_message>
cambios en la primer semana
</commit_message>
<xml_diff>
--- a/Plan_mes.xlsx
+++ b/Plan_mes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Programacion_del_mes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\UDEA\2do semestre\Informatica_2\Programacion_del_mes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423F9375-ABDA-454A-9D63-404C676F3E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C381CAE2-4586-4CCC-82D8-38ACE0890BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="68">
   <si>
     <t>Hora</t>
   </si>
@@ -223,6 +223,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Ingles</t>
+  </si>
+  <si>
+    <t>39h</t>
+  </si>
+  <si>
+    <t>Estudiar (algebra, info)</t>
   </si>
 </sst>
 </file>
@@ -294,7 +300,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -398,26 +404,270 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -429,67 +679,113 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -780,23 +1076,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="95" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" customWidth="1"/>
-    <col min="5" max="5" width="22.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1"/>
     <col min="6" max="6" width="19.88671875" customWidth="1"/>
     <col min="7" max="7" width="19.5546875" customWidth="1"/>
     <col min="8" max="8" width="20.33203125" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" customWidth="1"/>
-    <col min="11" max="11" width="24.77734375" customWidth="1"/>
+    <col min="10" max="10" width="17.21875" customWidth="1"/>
+    <col min="11" max="11" width="25.88671875" customWidth="1"/>
     <col min="12" max="12" width="23.77734375" customWidth="1"/>
     <col min="13" max="13" width="24.5546875" customWidth="1"/>
     <col min="14" max="14" width="21.21875" customWidth="1"/>
@@ -821,45 +1117,45 @@
   <sheetData>
     <row r="1" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
       <c r="Q1" s="1"/>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
       <c r="Y1" s="1"/>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="19"/>
+      <c r="AC1" s="19"/>
+      <c r="AD1" s="19"/>
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="19"/>
     </row>
     <row r="2" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -883,7 +1179,7 @@
       <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="60" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -963,589 +1259,587 @@
       <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="13" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="13" t="s">
+      <c r="E3" s="20"/>
+      <c r="F3" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="1" t="s">
+      <c r="G3" s="55"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="13" t="s">
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="13" t="s">
+      <c r="M3" s="20"/>
+      <c r="N3" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
       <c r="Q3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="13" t="s">
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="U3" s="2"/>
-      <c r="V3" s="13" t="s">
+      <c r="U3" s="20"/>
+      <c r="V3" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="23"/>
       <c r="Y3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="13" t="s">
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="13" t="s">
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="AE3" s="7"/>
-      <c r="AF3" s="7"/>
+      <c r="AE3" s="23"/>
+      <c r="AF3" s="23"/>
     </row>
     <row r="4" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="1" t="s">
+      <c r="B4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
       <c r="Q4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="24"/>
+      <c r="X4" s="24"/>
       <c r="Y4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="15"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="15"/>
-      <c r="AE4" s="8"/>
-      <c r="AF4" s="8"/>
+      <c r="Z4" s="20"/>
+      <c r="AA4" s="20"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="20"/>
+      <c r="AD4" s="22"/>
+      <c r="AE4" s="24"/>
+      <c r="AF4" s="24"/>
     </row>
     <row r="5" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="G5" s="56"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="L5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="M5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="N5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
       <c r="Q5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="R5" s="21" t="s">
+      <c r="R5" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="S5" s="13" t="s">
+      <c r="S5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="T5" s="10" t="s">
+      <c r="T5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="U5" s="13" t="s">
+      <c r="U5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="V5" s="10" t="s">
+      <c r="V5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="24"/>
       <c r="Y5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Z5" s="21" t="s">
+      <c r="Z5" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="AA5" s="13" t="s">
+      <c r="AA5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="AB5" s="10" t="s">
+      <c r="AB5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="AC5" s="13" t="s">
+      <c r="AC5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="AD5" s="10" t="s">
+      <c r="AD5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="AE5" s="8"/>
-      <c r="AF5" s="8"/>
+      <c r="AE5" s="24"/>
+      <c r="AF5" s="24"/>
     </row>
     <row r="6" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="1" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="22"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
       <c r="Q6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="R6" s="22"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="24"/>
+      <c r="X6" s="24"/>
       <c r="Y6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Z6" s="22"/>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="12"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="12"/>
-      <c r="AE6" s="8"/>
-      <c r="AF6" s="8"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="22"/>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="17"/>
+      <c r="AE6" s="24"/>
+      <c r="AF6" s="24"/>
     </row>
     <row r="7" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="10" t="s">
+      <c r="D7" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="20" t="s">
+      <c r="E7" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="27"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="J7" s="26"/>
-      <c r="K7" s="10" t="s">
+      <c r="J7" s="27"/>
+      <c r="K7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="23"/>
-      <c r="M7" s="10" t="s">
+      <c r="L7" s="10"/>
+      <c r="M7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="N7" s="26"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="20" t="s">
+      <c r="N7" s="27"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="R7" s="26"/>
-      <c r="S7" s="10" t="s">
+      <c r="R7" s="27"/>
+      <c r="S7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="T7" s="23"/>
-      <c r="U7" s="10" t="s">
+      <c r="T7" s="10"/>
+      <c r="U7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="V7" s="26"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="20" t="s">
+      <c r="V7" s="27"/>
+      <c r="W7" s="24"/>
+      <c r="X7" s="24"/>
+      <c r="Y7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="Z7" s="26"/>
-      <c r="AA7" s="10" t="s">
+      <c r="Z7" s="27"/>
+      <c r="AA7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="AB7" s="23"/>
-      <c r="AC7" s="10" t="s">
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="AD7" s="26"/>
-      <c r="AE7" s="8"/>
-      <c r="AF7" s="8"/>
+      <c r="AD7" s="27"/>
+      <c r="AE7" s="24"/>
+      <c r="AF7" s="24"/>
     </row>
     <row r="8" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="1" t="s">
+      <c r="B8" s="10"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="26"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
       <c r="Q8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="R8" s="26"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="24"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="26"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="27"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="24"/>
       <c r="Y8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Z8" s="26"/>
-      <c r="AA8" s="12"/>
-      <c r="AB8" s="24"/>
-      <c r="AC8" s="12"/>
-      <c r="AD8" s="26"/>
-      <c r="AE8" s="8"/>
-      <c r="AF8" s="8"/>
+      <c r="Z8" s="27"/>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="17"/>
+      <c r="AD8" s="27"/>
+      <c r="AE8" s="24"/>
+      <c r="AF8" s="24"/>
     </row>
     <row r="9" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="13" t="s">
+      <c r="D9" s="34"/>
+      <c r="E9" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="1" t="s">
+      <c r="F9" s="27"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="J9" s="26"/>
-      <c r="K9" s="13" t="s">
+      <c r="J9" s="27"/>
+      <c r="K9" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="24"/>
-      <c r="M9" s="13" t="s">
+      <c r="L9" s="11"/>
+      <c r="M9" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="N9" s="26"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
       <c r="Q9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="R9" s="26"/>
-      <c r="S9" s="13" t="s">
+      <c r="R9" s="27"/>
+      <c r="S9" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="T9" s="24"/>
-      <c r="U9" s="13" t="s">
+      <c r="T9" s="11"/>
+      <c r="U9" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="V9" s="26"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
+      <c r="V9" s="27"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="24"/>
       <c r="Y9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Z9" s="26"/>
-      <c r="AA9" s="13" t="s">
+      <c r="Z9" s="27"/>
+      <c r="AA9" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="AB9" s="24"/>
-      <c r="AC9" s="13" t="s">
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="AD9" s="26"/>
-      <c r="AE9" s="8"/>
-      <c r="AF9" s="8"/>
+      <c r="AD9" s="27"/>
+      <c r="AE9" s="24"/>
+      <c r="AF9" s="24"/>
     </row>
     <row r="10" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="1" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="J10" s="26"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
       <c r="Q10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="R10" s="26"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="24"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="26"/>
-      <c r="W10" s="8"/>
-      <c r="X10" s="8"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="22"/>
+      <c r="V10" s="27"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
       <c r="Y10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Z10" s="26"/>
-      <c r="AA10" s="15"/>
-      <c r="AB10" s="24"/>
-      <c r="AC10" s="15"/>
-      <c r="AD10" s="26"/>
-      <c r="AE10" s="8"/>
-      <c r="AF10" s="8"/>
+      <c r="Z10" s="27"/>
+      <c r="AA10" s="22"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="22"/>
+      <c r="AD10" s="27"/>
+      <c r="AE10" s="24"/>
+      <c r="AF10" s="24"/>
     </row>
     <row r="11" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="29" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="27" t="s">
+      <c r="E11" s="10"/>
+      <c r="F11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="1" t="s">
+      <c r="G11" s="56"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="K11" s="23"/>
+      <c r="K11" s="10"/>
       <c r="L11" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="M11" s="23"/>
-      <c r="N11" s="27" t="s">
+      <c r="M11" s="10"/>
+      <c r="N11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O11" s="9"/>
-      <c r="P11" s="8"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="24"/>
       <c r="Q11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="R11" s="13" t="s">
+      <c r="R11" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="S11" s="23"/>
+      <c r="S11" s="10"/>
       <c r="T11" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="U11" s="23"/>
-      <c r="V11" s="27" t="s">
+      <c r="U11" s="10"/>
+      <c r="V11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="W11" s="9"/>
-      <c r="X11" s="8"/>
+      <c r="W11" s="25"/>
+      <c r="X11" s="24"/>
       <c r="Y11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Z11" s="13" t="s">
+      <c r="Z11" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="AA11" s="23"/>
+      <c r="AA11" s="10"/>
       <c r="AB11" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="AC11" s="23"/>
-      <c r="AD11" s="27" t="s">
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="AE11" s="9"/>
-      <c r="AF11" s="8"/>
+      <c r="AE11" s="25"/>
+      <c r="AF11" s="24"/>
     </row>
     <row r="12" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="10" t="s">
+      <c r="B12" s="28"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="61"/>
+      <c r="I12" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="28"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J12" s="14"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="P12" s="9"/>
+      <c r="P12" s="25"/>
       <c r="Q12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="R12" s="14"/>
-      <c r="S12" s="24"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="11"/>
       <c r="T12" s="29"/>
-      <c r="U12" s="24"/>
-      <c r="V12" s="28"/>
-      <c r="W12" s="10" t="s">
+      <c r="U12" s="11"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="X12" s="9"/>
+      <c r="X12" s="25"/>
       <c r="Y12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Z12" s="14"/>
-      <c r="AA12" s="24"/>
+      <c r="Z12" s="28"/>
+      <c r="AA12" s="11"/>
       <c r="AB12" s="29"/>
-      <c r="AC12" s="24"/>
-      <c r="AD12" s="28"/>
-      <c r="AE12" s="10" t="s">
+      <c r="AC12" s="11"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="AF12" s="9"/>
+      <c r="AF12" s="25"/>
     </row>
     <row r="13" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="B13" s="22"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="J13" s="15"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="10" t="s">
+      <c r="J13" s="22"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="13" t="s">
         <v>25</v>
       </c>
       <c r="Q13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="R13" s="15"/>
-      <c r="S13" s="25"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="25"/>
-      <c r="V13" s="23"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="10" t="s">
+      <c r="R13" s="22"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="14"/>
+      <c r="X13" s="13" t="s">
         <v>25</v>
       </c>
       <c r="Y13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="Z13" s="15"/>
-      <c r="AA13" s="25"/>
-      <c r="AB13" s="23"/>
-      <c r="AC13" s="25"/>
-      <c r="AD13" s="23"/>
-      <c r="AE13" s="11"/>
-      <c r="AF13" s="10" t="s">
+      <c r="Z13" s="22"/>
+      <c r="AA13" s="12"/>
+      <c r="AB13" s="10"/>
+      <c r="AC13" s="12"/>
+      <c r="AD13" s="10"/>
+      <c r="AE13" s="14"/>
+      <c r="AF13" s="13" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1553,467 +1847,471 @@
       <c r="A14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="10" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="34"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="10" t="s">
+      <c r="L14" s="11"/>
+      <c r="M14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J14" s="23"/>
-      <c r="K14" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="L14" s="24"/>
-      <c r="M14" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="N14" s="24"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
       <c r="Q14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="R14" s="23"/>
-      <c r="S14" s="10" t="s">
+      <c r="R14" s="10"/>
+      <c r="S14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="T14" s="24"/>
-      <c r="U14" s="10" t="s">
+      <c r="T14" s="11"/>
+      <c r="U14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="V14" s="24"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
       <c r="Y14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="Z14" s="23"/>
-      <c r="AA14" s="10" t="s">
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="AB14" s="24"/>
-      <c r="AC14" s="10" t="s">
+      <c r="AB14" s="11"/>
+      <c r="AC14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="AD14" s="24"/>
-      <c r="AE14" s="11"/>
-      <c r="AF14" s="11"/>
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="14"/>
+      <c r="AF14" s="14"/>
     </row>
     <row r="15" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="1" t="s">
+      <c r="B15" s="11"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="J15" s="24"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
       <c r="Q15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="R15" s="24"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="25"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
       <c r="Y15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Z15" s="24"/>
-      <c r="AA15" s="11"/>
-      <c r="AB15" s="25"/>
-      <c r="AC15" s="11"/>
-      <c r="AD15" s="24"/>
-      <c r="AE15" s="11"/>
-      <c r="AF15" s="11"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="14"/>
+      <c r="AB15" s="12"/>
+      <c r="AC15" s="14"/>
+      <c r="AD15" s="11"/>
+      <c r="AE15" s="14"/>
+      <c r="AF15" s="14"/>
     </row>
     <row r="16" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="10" t="s">
+      <c r="B16" s="39"/>
+      <c r="C16" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="3" t="s">
+      <c r="E16" s="15"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="J16" s="12"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="14"/>
+      <c r="N16" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J16" s="25"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="M16" s="11"/>
-      <c r="N16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
       <c r="Q16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="R16" s="25"/>
-      <c r="S16" s="22"/>
-      <c r="T16" s="10" t="s">
+      <c r="R16" s="12"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="U16" s="11"/>
-      <c r="V16" s="3" t="s">
+      <c r="U16" s="14"/>
+      <c r="V16" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="W16" s="11"/>
-      <c r="X16" s="11"/>
+      <c r="W16" s="14"/>
+      <c r="X16" s="14"/>
       <c r="Y16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="Z16" s="25"/>
-      <c r="AA16" s="22"/>
-      <c r="AB16" s="10" t="s">
+      <c r="Z16" s="12"/>
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="AC16" s="11"/>
-      <c r="AD16" s="3" t="s">
+      <c r="AC16" s="14"/>
+      <c r="AD16" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="AE16" s="11"/>
-      <c r="AF16" s="11"/>
+      <c r="AE16" s="14"/>
+      <c r="AF16" s="14"/>
     </row>
     <row r="17" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="49"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="J17" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="22"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
       <c r="Q17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="R17" s="10" t="s">
+      <c r="R17" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="S17" s="22"/>
-      <c r="T17" s="11"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="3"/>
-      <c r="W17" s="11"/>
-      <c r="X17" s="11"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="14"/>
+      <c r="V17" s="18"/>
+      <c r="W17" s="14"/>
+      <c r="X17" s="14"/>
       <c r="Y17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="Z17" s="10" t="s">
+      <c r="Z17" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="AA17" s="22"/>
-      <c r="AB17" s="11"/>
-      <c r="AC17" s="11"/>
-      <c r="AD17" s="3"/>
-      <c r="AE17" s="11"/>
-      <c r="AF17" s="11"/>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="14"/>
+      <c r="AC17" s="14"/>
+      <c r="AD17" s="18"/>
+      <c r="AE17" s="14"/>
+      <c r="AF17" s="14"/>
     </row>
     <row r="18" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="1" t="s">
+      <c r="B18" s="16"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="J18" s="12"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="12"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="17"/>
       <c r="Q18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="R18" s="12"/>
-      <c r="S18" s="30"/>
-      <c r="T18" s="11"/>
-      <c r="U18" s="12"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="11"/>
-      <c r="X18" s="12"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="18"/>
+      <c r="W18" s="14"/>
+      <c r="X18" s="17"/>
       <c r="Y18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="Z18" s="12"/>
-      <c r="AA18" s="30"/>
-      <c r="AB18" s="11"/>
-      <c r="AC18" s="12"/>
-      <c r="AD18" s="3"/>
-      <c r="AE18" s="11"/>
-      <c r="AF18" s="12"/>
+      <c r="Z18" s="17"/>
+      <c r="AA18" s="16"/>
+      <c r="AB18" s="14"/>
+      <c r="AC18" s="17"/>
+      <c r="AD18" s="18"/>
+      <c r="AE18" s="14"/>
+      <c r="AF18" s="17"/>
     </row>
     <row r="19" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="1" t="s">
+      <c r="B19" s="46"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="26"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="27"/>
       <c r="Q19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="R19" s="26"/>
-      <c r="S19" s="26"/>
-      <c r="T19" s="12"/>
-      <c r="U19" s="26"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="12"/>
+      <c r="R19" s="27"/>
+      <c r="S19" s="27"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="27"/>
+      <c r="V19" s="18"/>
+      <c r="W19" s="17"/>
       <c r="X19" s="31"/>
       <c r="Y19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="Z19" s="26"/>
-      <c r="AA19" s="26"/>
-      <c r="AB19" s="12"/>
-      <c r="AC19" s="26"/>
-      <c r="AD19" s="3"/>
-      <c r="AE19" s="12"/>
-      <c r="AF19" s="26"/>
+      <c r="Z19" s="27"/>
+      <c r="AA19" s="27"/>
+      <c r="AB19" s="17"/>
+      <c r="AC19" s="27"/>
+      <c r="AD19" s="18"/>
+      <c r="AE19" s="17"/>
+      <c r="AF19" s="27"/>
     </row>
     <row r="20" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="1" t="s">
+      <c r="B20" s="46"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="23"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="10"/>
       <c r="O20" s="31"/>
-      <c r="P20" s="26"/>
+      <c r="P20" s="27"/>
       <c r="Q20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="R20" s="26"/>
-      <c r="S20" s="26"/>
-      <c r="T20" s="26"/>
-      <c r="U20" s="26"/>
-      <c r="V20" s="26"/>
-      <c r="W20" s="26"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="27"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="27"/>
       <c r="X20" s="31"/>
       <c r="Y20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="Z20" s="26"/>
-      <c r="AA20" s="26"/>
-      <c r="AB20" s="26"/>
-      <c r="AC20" s="26"/>
-      <c r="AD20" s="26"/>
-      <c r="AE20" s="26"/>
-      <c r="AF20" s="26"/>
+      <c r="Z20" s="27"/>
+      <c r="AA20" s="27"/>
+      <c r="AB20" s="27"/>
+      <c r="AC20" s="27"/>
+      <c r="AD20" s="27"/>
+      <c r="AE20" s="27"/>
+      <c r="AF20" s="27"/>
     </row>
     <row r="21" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="1" t="s">
+      <c r="B21" s="46"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="24"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="11"/>
       <c r="O21" s="31"/>
-      <c r="P21" s="26"/>
+      <c r="P21" s="27"/>
       <c r="Q21" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="R21" s="26"/>
-      <c r="S21" s="26"/>
-      <c r="T21" s="26"/>
-      <c r="U21" s="26"/>
-      <c r="V21" s="26"/>
-      <c r="W21" s="26"/>
+      <c r="R21" s="27"/>
+      <c r="S21" s="27"/>
+      <c r="T21" s="27"/>
+      <c r="U21" s="27"/>
+      <c r="V21" s="27"/>
+      <c r="W21" s="27"/>
       <c r="X21" s="31"/>
       <c r="Y21" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="Z21" s="26"/>
-      <c r="AA21" s="26"/>
-      <c r="AB21" s="26"/>
-      <c r="AC21" s="26"/>
-      <c r="AD21" s="26"/>
-      <c r="AE21" s="26"/>
-      <c r="AF21" s="26"/>
+      <c r="Z21" s="27"/>
+      <c r="AA21" s="27"/>
+      <c r="AB21" s="27"/>
+      <c r="AC21" s="27"/>
+      <c r="AD21" s="27"/>
+      <c r="AE21" s="27"/>
+      <c r="AF21" s="27"/>
     </row>
     <row r="22" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="1" t="s">
+      <c r="B22" s="46"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="24"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="11"/>
       <c r="O22" s="31"/>
-      <c r="P22" s="26"/>
+      <c r="P22" s="27"/>
       <c r="Q22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="R22" s="26"/>
-      <c r="S22" s="26"/>
-      <c r="T22" s="26"/>
-      <c r="U22" s="26"/>
-      <c r="V22" s="26"/>
-      <c r="W22" s="26"/>
+      <c r="R22" s="27"/>
+      <c r="S22" s="27"/>
+      <c r="T22" s="27"/>
+      <c r="U22" s="27"/>
+      <c r="V22" s="27"/>
+      <c r="W22" s="27"/>
       <c r="X22" s="31"/>
       <c r="Y22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="Z22" s="26"/>
-      <c r="AA22" s="26"/>
-      <c r="AB22" s="26"/>
-      <c r="AC22" s="26"/>
-      <c r="AD22" s="26"/>
-      <c r="AE22" s="26"/>
-      <c r="AF22" s="26"/>
+      <c r="Z22" s="27"/>
+      <c r="AA22" s="27"/>
+      <c r="AB22" s="27"/>
+      <c r="AC22" s="27"/>
+      <c r="AD22" s="27"/>
+      <c r="AE22" s="27"/>
+      <c r="AF22" s="27"/>
     </row>
     <row r="23" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="1" t="s">
+      <c r="B23" s="46"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="25"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="12"/>
       <c r="O23" s="31"/>
-      <c r="P23" s="26"/>
+      <c r="P23" s="27"/>
       <c r="Q23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="R23" s="26"/>
-      <c r="S23" s="26"/>
-      <c r="T23" s="26"/>
-      <c r="U23" s="26"/>
-      <c r="V23" s="26"/>
-      <c r="W23" s="26"/>
+      <c r="R23" s="27"/>
+      <c r="S23" s="27"/>
+      <c r="T23" s="27"/>
+      <c r="U23" s="27"/>
+      <c r="V23" s="27"/>
+      <c r="W23" s="27"/>
       <c r="X23" s="31"/>
       <c r="Y23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Z23" s="26"/>
-      <c r="AA23" s="26"/>
-      <c r="AB23" s="26"/>
-      <c r="AC23" s="26"/>
-      <c r="AD23" s="26"/>
-      <c r="AE23" s="26"/>
-      <c r="AF23" s="26"/>
+      <c r="Z23" s="27"/>
+      <c r="AA23" s="27"/>
+      <c r="AB23" s="27"/>
+      <c r="AC23" s="27"/>
+      <c r="AD23" s="27"/>
+      <c r="AE23" s="27"/>
+      <c r="AF23" s="27"/>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="2" t="s">
         <v>27</v>
       </c>
       <c r="H25" t="s">
@@ -2022,21 +2320,21 @@
       <c r="J25" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="17" t="s">
+      <c r="L25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M25" s="16"/>
+      <c r="M25" s="2"/>
       <c r="R25" t="s">
         <v>37</v>
       </c>
-      <c r="T25" s="17" t="s">
+      <c r="T25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="V25" s="17"/>
+      <c r="V25" s="3"/>
       <c r="Z25" t="s">
         <v>41</v>
       </c>
-      <c r="AB25" s="17" t="s">
+      <c r="AB25" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2044,6 +2342,9 @@
       <c r="B26" t="s">
         <v>28</v>
       </c>
+      <c r="D26" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="J26" t="s">
         <v>34</v>
       </c>
@@ -2058,26 +2359,26 @@
       <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="3" t="s">
         <v>31</v>
       </c>
       <c r="J27" t="s">
         <v>35</v>
       </c>
-      <c r="L27" s="17" t="s">
+      <c r="L27" s="3" t="s">
         <v>31</v>
       </c>
       <c r="R27" t="s">
         <v>39</v>
       </c>
-      <c r="T27" s="16" t="s">
+      <c r="T27" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="V27" s="16"/>
+      <c r="V27" s="2"/>
       <c r="Z27" t="s">
         <v>43</v>
       </c>
-      <c r="AB27" s="16" t="s">
+      <c r="AB27" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2085,6 +2386,9 @@
       <c r="B28" t="s">
         <v>32</v>
       </c>
+      <c r="D28" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="J28" t="s">
         <v>36</v>
       </c>
@@ -2096,12 +2400,18 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="168">
-    <mergeCell ref="H19:H23"/>
-    <mergeCell ref="G20:G23"/>
+  <mergeCells count="169">
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="G17:G20"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="H17:H20"/>
+    <mergeCell ref="H3:H13"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="F13:F23"/>
     <mergeCell ref="E19:E23"/>
     <mergeCell ref="D20:D23"/>
-    <mergeCell ref="C19:C23"/>
     <mergeCell ref="B19:B23"/>
     <mergeCell ref="Z17:Z18"/>
     <mergeCell ref="AF19:AF23"/>
@@ -2111,8 +2421,17 @@
     <mergeCell ref="AB20:AB23"/>
     <mergeCell ref="AA19:AA23"/>
     <mergeCell ref="Z19:Z23"/>
-    <mergeCell ref="R7:R10"/>
-    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="L20:L23"/>
+    <mergeCell ref="AF13:AF18"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="M14:M18"/>
+    <mergeCell ref="N16:N19"/>
+    <mergeCell ref="P19:P23"/>
+    <mergeCell ref="O20:O23"/>
+    <mergeCell ref="N20:N23"/>
+    <mergeCell ref="M19:M23"/>
     <mergeCell ref="T7:T10"/>
     <mergeCell ref="U7:U8"/>
     <mergeCell ref="V7:V10"/>
@@ -2159,57 +2478,41 @@
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="F7:F10"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F20:F23"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="E11:E13"/>
     <mergeCell ref="E14:E18"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="F16:F19"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B13"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="G3:G11"/>
-    <mergeCell ref="G12:G19"/>
-    <mergeCell ref="H3:H12"/>
-    <mergeCell ref="H13:H18"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D9:D10"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="J14:J16"/>
     <mergeCell ref="K14:K18"/>
     <mergeCell ref="L16:L19"/>
     <mergeCell ref="J17:J18"/>
-    <mergeCell ref="L20:L23"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="M3:M4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="M14:M18"/>
-    <mergeCell ref="N16:N19"/>
-    <mergeCell ref="P19:P23"/>
-    <mergeCell ref="O20:O23"/>
-    <mergeCell ref="N20:N23"/>
-    <mergeCell ref="M19:M23"/>
+    <mergeCell ref="D3:D4"/>
     <mergeCell ref="K19:K23"/>
     <mergeCell ref="J19:J23"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="G3:G11"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B11:B13"/>
     <mergeCell ref="R1:X1"/>
     <mergeCell ref="S3:S4"/>
     <mergeCell ref="U3:U4"/>
@@ -2231,6 +2534,9 @@
     <mergeCell ref="T20:T23"/>
     <mergeCell ref="S19:S23"/>
     <mergeCell ref="R19:R23"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="R7:R10"/>
+    <mergeCell ref="S7:S8"/>
     <mergeCell ref="Z1:AF1"/>
     <mergeCell ref="Z3:Z4"/>
     <mergeCell ref="AA3:AA4"/>
@@ -2264,7 +2570,6 @@
     <mergeCell ref="AB16:AB19"/>
     <mergeCell ref="AD16:AD19"/>
     <mergeCell ref="AE12:AE19"/>
-    <mergeCell ref="AF13:AF18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>